<commit_message>
falta solo los botones de liberacion
</commit_message>
<xml_diff>
--- a/src/assets/PLANTILLA_VIAJE.xlsx
+++ b/src/assets/PLANTILLA_VIAJE.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\REIM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leogh\Documents\GitHub\REIMFront\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{855A4043-8ACE-4B37-9151-1633118C2952}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9195"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="2" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Viaje</t>
   </si>
@@ -37,12 +38,15 @@
   </si>
   <si>
     <t>Buque</t>
+  </si>
+  <si>
+    <t>Patio</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -360,11 +364,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -376,7 +380,7 @@
     <col min="6" max="6" width="14.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -394,6 +398,9 @@
       </c>
       <c r="F1" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>